<commit_message>
Second commit with new files
</commit_message>
<xml_diff>
--- a/ExcelData.xlsx
+++ b/ExcelData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\UiPath\Resume-Generator-Bot-UiPath-RPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\UiPath\ResumeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AFB8F2-0255-4E9D-9960-62112A94AB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55876453-7A3C-4C00-94B6-58F3EEE6F8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="80">
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Abhishek Kusalkar</t>
-  </si>
-  <si>
-    <t>Pawan Gade</t>
   </si>
   <si>
     <t>Role</t>
@@ -252,10 +246,28 @@
     <t>HardWork</t>
   </si>
   <si>
-    <t>linkedin/abhishek</t>
-  </si>
-  <si>
-    <t>linkedlin/pawan</t>
+    <t>4 Months</t>
+  </si>
+  <si>
+    <t>Profile3</t>
+  </si>
+  <si>
+    <t>linkedin/varun</t>
+  </si>
+  <si>
+    <t>linkedlin/ayisha</t>
+  </si>
+  <si>
+    <t>linkedlin/kavya</t>
+  </si>
+  <si>
+    <t>Varun Chowdary Vankayalapati</t>
+  </si>
+  <si>
+    <t>Kavya Sree Bandi</t>
+  </si>
+  <si>
+    <t>Ayisha Sadiq Shaik</t>
   </si>
 </sst>
 </file>
@@ -616,15 +628,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM3"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
@@ -666,180 +678,180 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM1" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
       <c r="C2">
         <v>9370255282</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>31</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
         <v>33</v>
       </c>
-      <c r="O2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
         <v>37</v>
-      </c>
-      <c r="S2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" t="s">
-        <v>39</v>
       </c>
       <c r="U2">
         <v>2024</v>
@@ -848,22 +860,22 @@
         <v>8.56</v>
       </c>
       <c r="W2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" t="s">
         <v>44</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>45</v>
       </c>
-      <c r="Y2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>47</v>
-      </c>
       <c r="AA2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AC2">
         <v>2020</v>
@@ -872,93 +884,93 @@
         <v>70</v>
       </c>
       <c r="AE2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AF2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AG2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM2" t="s">
         <v>71</v>
       </c>
-      <c r="AH2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>73</v>
-      </c>
     </row>
-    <row r="3" spans="1:39" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>9370255282</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>30</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>31</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>32</v>
       </c>
-      <c r="N3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" t="s">
         <v>34</v>
       </c>
-      <c r="P3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="R3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="T3" t="s">
         <v>37</v>
-      </c>
-      <c r="S3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" t="s">
-        <v>39</v>
       </c>
       <c r="U3">
         <v>2024</v>
@@ -967,22 +979,22 @@
         <v>9.4499999999999993</v>
       </c>
       <c r="W3" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y3" t="s">
         <v>44</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>45</v>
       </c>
-      <c r="Y3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>47</v>
-      </c>
       <c r="AA3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AC3">
         <v>2020</v>
@@ -991,31 +1003,150 @@
         <v>70</v>
       </c>
       <c r="AE3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>9370255283</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" t="s">
         <v>36</v>
       </c>
-      <c r="AG3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI3" t="s">
+      <c r="T4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4">
+        <v>2024</v>
+      </c>
+      <c r="V4">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="W4" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC4">
+        <v>2020</v>
+      </c>
+      <c r="AD4">
+        <v>70</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK4" t="s">
         <v>64</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM3" t="s">
+      <c r="AL4" t="s">
         <v>73</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1025,8 +1156,10 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{9BAE8D6C-7DD1-4F9C-A4A4-1BF50711DF70}"/>
     <hyperlink ref="E2" r:id="rId3" display="https://www.linkedin.com/abhishek" xr:uid="{B5595699-55F3-4055-94E9-D54D7DC4BBCA}"/>
     <hyperlink ref="E3" r:id="rId4" display="https://www.linkedin.com/abhishek" xr:uid="{F7EFAA1B-6778-4FE2-900E-B0BD19E7BBBD}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{E87BD62A-4BF7-42CF-A938-2FAC329C5B7A}"/>
+    <hyperlink ref="E4" r:id="rId6" display="https://www.linkedin.com/abhishek" xr:uid="{092AB98D-C462-46B5-8787-0CB696423982}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>